<commit_message>
Did a bit more on cookies off / on graph sections
</commit_message>
<xml_diff>
--- a/TB2/Duration Plots using TCPDump.xlsx
+++ b/TB2/Duration Plots using TCPDump.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -27,8 +27,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,12 +65,27 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -88,1194 +103,1232 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38268312727453846"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$185</c:f>
+              <c:f>Sheet1!$A$3:$A$185</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="184"/>
+                <c:ptCount val="183"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>54</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>59</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>61</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>62</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>64</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>66</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>67</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>68</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>69</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>70</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>71</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>72</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>73</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>74</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>75</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>76</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>77</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>78</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>79</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>80</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>81</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>82</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>83</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>84</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>85</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>86</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>87</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>88</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>89</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>90</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>91</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>92</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>93</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>94</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>95</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>96</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>97</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>98</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>99</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>100</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>101</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>102</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>103</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>104</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>105</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>106</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>108</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>109</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>110</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>111</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>112</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>113</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>115</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>116</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>117</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>118</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>119</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>121</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>122</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>123</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>124</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>125</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>126</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>127</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>128</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>129</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>130</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>131</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>132</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>133</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>134</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>135</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>136</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>137</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>138</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>139</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>140</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>141</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>142</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>143</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>144</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>145</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>146</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>147</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>148</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>149</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>150</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>151</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>152</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>153</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>155</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>156</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>157</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>158</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>159</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>160</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>161</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>162</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>163</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>164</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>165</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>166</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>167</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>168</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>169</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>170</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>171</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>172</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>173</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>174</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>175</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>176</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>177</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>178</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>179</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>181</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>182</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>183</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>184</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>185</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>186</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>187</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="183">
                   <c:v>189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$185</c:f>
+              <c:f>Sheet1!$B$3:$B$185</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="184"/>
+                <c:ptCount val="183"/>
+                <c:pt idx="0">
+                  <c:v>8444</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>8444</c:v>
+                  <c:v>7247</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>7080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6953</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6971</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7539</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7285</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6859</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7056</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7032</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7011</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7262</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7229</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6962</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7040</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6973</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7281</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7035</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6992</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7173</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6982</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7061</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6945</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7060</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6755</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7333</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6769</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6901</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6879</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6676</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6581</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7103</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7116</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6809</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7061</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6944</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6748</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7030</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6710</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6766</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7133</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6897</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6504</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6893</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6862</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6836</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7062</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6575</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6766</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7056</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7149</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6919</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6719</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6679</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6795</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7082</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6756</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6726</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6897</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7006</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6823</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6790</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6981</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7080</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6954</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6843</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7107</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6941</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6906</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6758</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6841</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6906</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6755</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6888</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>7021</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6630</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6811</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6725</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6675</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6756</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6732</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6714</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7084</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6833</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6736</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7185</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6969</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6539</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6730</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6860</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6912</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6856</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>6866</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6887</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>6796</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7020</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>7189</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>6902</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>6856</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>6836</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>7126</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>6847</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>7196</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>6946</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>6754</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>6790</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>6733</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>7168</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>6823</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>7133</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>6815</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>6756</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>7132</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>7011</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>6637</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>7683</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6884</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>6750</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>7174</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>6640</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>6868</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6812</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>6809</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>7070</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>6868</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>7152</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>7066</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>7483</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>7244</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>6991</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>6598</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>7201</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>6777</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>7850</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>7051</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>7113</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>7060</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>7111</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>6901</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7505</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>6654</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>7165</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>6760</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>7232</c:v>
+                </c:pt>
+                <c:pt idx="154">
                   <c:v>7247</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7080</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7238</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6953</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6951</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6971</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7539</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7053</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7285</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6859</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7056</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7032</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7011</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7262</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7207</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7304</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7229</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8005</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6962</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7040</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6973</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="155">
+                  <c:v>7260</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>7012</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>7086</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>7315</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>7198</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>7549</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>7249</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>7316</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>6978</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>7187</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>7346</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>6984</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>7743</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>6995</c:v>
+                </c:pt>
+                <c:pt idx="169">
                   <c:v>7281</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>7035</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6992</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7173</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6982</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="170">
+                  <c:v>6991</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>7004</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>6950</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>7002</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="175">
                   <c:v>7061</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>6945</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>6995</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7060</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6755</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7333</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6769</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6901</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6879</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6676</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6581</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7103</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>7116</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6809</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>7061</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6944</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>6748</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7030</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>6710</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6766</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>7133</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>6897</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>6504</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6893</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6862</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6836</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>7062</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6575</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6766</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>7056</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>7149</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>6919</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6719</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6679</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>7002</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6795</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>7082</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6756</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6726</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6897</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>7006</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>6690</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>6823</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>6790</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>6981</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7080</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>6954</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>6843</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7107</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>6941</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>6906</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>6758</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>6841</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>6906</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>6755</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>6888</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>7021</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>6630</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>6811</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>6725</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>6675</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>6756</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>6732</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>6714</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>7084</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>6833</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>6736</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>7185</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>6969</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>6539</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>6730</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>6860</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>6912</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>6856</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>6866</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>6887</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>6796</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>7020</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>7189</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>6902</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>6856</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>6836</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>7126</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>6847</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>7196</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>6946</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>6754</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>6790</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>6733</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>7168</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>6823</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>7133</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>6815</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>6756</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>7132</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>7011</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>6637</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>7683</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>6884</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>6750</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>7174</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>6640</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>6868</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>6812</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>6809</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>7070</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>6868</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7152</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7066</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>7483</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7244</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>6991</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>6598</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>7201</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>6777</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>7850</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>7051</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>7113</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>7060</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>7111</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>6901</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>7505</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>6654</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>7165</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>6760</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>7232</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7247</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>7260</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>7012</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>7086</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>7315</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>7198</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>7549</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>7249</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>7316</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>6978</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>7187</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>7346</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>6984</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>7743</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>6995</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>7281</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>6991</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>7004</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>6950</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>7002</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>7028</c:v>
-                </c:pt>
                 <c:pt idx="176">
-                  <c:v>7061</c:v>
+                  <c:v>6957</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>6957</c:v>
+                  <c:v>7245</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>7245</c:v>
+                  <c:v>7063</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>7063</c:v>
+                  <c:v>6947</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>6947</c:v>
+                  <c:v>7939</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>7939</c:v>
+                  <c:v>6956</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>6956</c:v>
-                </c:pt>
-                <c:pt idx="183">
                   <c:v>7206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92302336"/>
-        <c:axId val="101183872"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="92302336"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="59532800"/>
+        <c:axId val="59531264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="59532800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="l"/>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101183872"/>
+        <c:crossAx val="59531264"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="101183872"/>
+        <c:axId val="59531264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="b"/>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Duration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92302336"/>
+        <c:crossAx val="59532800"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1287,7 +1340,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1306,431 +1369,463 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$185</c:f>
+              <c:f>Sheet1!$C$3:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="184"/>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>94</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>159</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>161</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>162</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>163</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>164</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>165</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>166</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>167</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>168</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>169</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>170</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>171</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>172</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>173</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>174</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>175</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>176</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>177</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>178</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>180</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>181</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>182</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>183</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>184</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="56">
                   <c:v>186</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$185</c:f>
+              <c:f>Sheet1!$D$3:$D$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="184"/>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>7393</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>7393</c:v>
+                  <c:v>6990</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6928</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6829</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7311</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>6990</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>6883</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6928</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6829</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7311</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>6990</c:v>
+                  <c:v>7060</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7060</c:v>
+                  <c:v>7011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7011</c:v>
+                  <c:v>7566</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7566</c:v>
+                  <c:v>6981</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6981</c:v>
+                  <c:v>7012</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7012</c:v>
+                  <c:v>7272</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7272</c:v>
+                  <c:v>7506</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7506</c:v>
+                  <c:v>6996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6996</c:v>
+                  <c:v>7079</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7079</c:v>
+                  <c:v>7005</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>7225</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7638</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7458</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7052</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7222</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7019</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7034</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7089</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7069</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7282</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7277</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8994</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8434</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7015</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7242</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7159</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7495</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6945</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7356</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7252</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6993</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7018</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6985</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6992</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7063</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7185</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7217</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7316</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>7005</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>7225</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7638</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7458</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7052</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7222</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7019</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7034</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7089</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7069</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7282</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7277</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8994</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8434</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7015</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7242</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7159</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7495</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7028</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6945</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7356</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7252</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6993</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>7018</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6985</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>6992</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>7063</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>7185</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7217</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7316</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>7005</c:v>
+                  <c:v>7240</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7240</c:v>
+                  <c:v>7250</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7250</c:v>
+                  <c:v>6944</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6944</c:v>
+                  <c:v>7270</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7270</c:v>
+                  <c:v>7111</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7111</c:v>
+                  <c:v>6951</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6951</c:v>
+                  <c:v>7112</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7112</c:v>
-                </c:pt>
-                <c:pt idx="56">
                   <c:v>7049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="101683584"/>
-        <c:axId val="101685120"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="101683584"/>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="43736064"/>
+        <c:axId val="43734528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="43736064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="l"/>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101685120"/>
+        <c:crossAx val="43734528"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="101685120"/>
+        <c:axId val="43734528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="b"/>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Duration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101683584"/>
+        <c:crossAx val="43736064"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1744,20 +1839,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>140804</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>181389</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>422412</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>67089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1774,20 +1869,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>538370</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>132523</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>40584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>16566</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438978</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>116784</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1880,6 +1975,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1914,6 +2010,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2089,16 +2186,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2126,7 +2223,7 @@
         <v>7393</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2140,7 +2237,7 @@
         <v>6990</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2154,7 +2251,7 @@
         <v>6883</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2168,7 +2265,7 @@
         <v>6928</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2182,7 +2279,7 @@
         <v>6829</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2196,7 +2293,7 @@
         <v>7311</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2210,7 +2307,7 @@
         <v>6990</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2224,7 +2321,7 @@
         <v>7060</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2238,7 +2335,7 @@
         <v>7011</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2252,7 +2349,7 @@
         <v>7566</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2266,7 +2363,7 @@
         <v>6981</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2280,7 +2377,7 @@
         <v>7012</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2294,7 +2391,7 @@
         <v>7272</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2308,7 +2405,7 @@
         <v>7506</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2322,7 +2419,7 @@
         <v>6996</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2336,7 +2433,7 @@
         <v>7079</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2350,7 +2447,7 @@
         <v>7005</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2364,7 +2461,7 @@
         <v>7225</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2378,7 +2475,7 @@
         <v>7638</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2392,7 +2489,7 @@
         <v>7458</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2406,7 +2503,7 @@
         <v>7052</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2420,7 +2517,7 @@
         <v>7222</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2434,7 +2531,7 @@
         <v>7019</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2448,7 +2545,7 @@
         <v>7034</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2462,7 +2559,7 @@
         <v>7089</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2476,7 +2573,7 @@
         <v>7004</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2490,7 +2587,7 @@
         <v>7069</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2504,7 +2601,7 @@
         <v>7282</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2518,7 +2615,7 @@
         <v>7277</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2532,7 +2629,7 @@
         <v>8994</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2546,7 +2643,7 @@
         <v>8434</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2560,7 +2657,7 @@
         <v>7015</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2574,7 +2671,7 @@
         <v>7242</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2588,7 +2685,7 @@
         <v>7159</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2602,7 +2699,7 @@
         <v>7495</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2616,7 +2713,7 @@
         <v>7028</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2630,7 +2727,7 @@
         <v>6945</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2644,7 +2741,7 @@
         <v>7356</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2658,7 +2755,7 @@
         <v>7252</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2672,7 +2769,7 @@
         <v>6993</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2686,7 +2783,7 @@
         <v>7018</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2700,7 +2797,7 @@
         <v>6985</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2714,7 +2811,7 @@
         <v>6992</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2728,7 +2825,7 @@
         <v>7063</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2742,7 +2839,7 @@
         <v>7185</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2756,7 +2853,7 @@
         <v>7217</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2770,7 +2867,7 @@
         <v>7316</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2784,7 +2881,7 @@
         <v>7005</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2798,7 +2895,7 @@
         <v>7240</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2812,7 +2909,7 @@
         <v>7250</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2826,7 +2923,7 @@
         <v>6944</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2840,7 +2937,7 @@
         <v>7270</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2854,7 +2951,7 @@
         <v>7111</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2868,7 +2965,7 @@
         <v>6951</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2882,7 +2979,7 @@
         <v>7112</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2896,7 +2993,7 @@
         <v>7049</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2904,7 +3001,7 @@
         <v>6766</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2912,7 +3009,7 @@
         <v>7056</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2920,7 +3017,7 @@
         <v>7149</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2928,7 +3025,7 @@
         <v>6919</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2936,7 +3033,7 @@
         <v>6719</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2944,7 +3041,7 @@
         <v>6679</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2952,7 +3049,7 @@
         <v>7002</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
@@ -2960,7 +3057,7 @@
         <v>6795</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
@@ -2968,7 +3065,7 @@
         <v>7082</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
@@ -2976,7 +3073,7 @@
         <v>6756</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
@@ -2984,7 +3081,7 @@
         <v>6726</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
@@ -2992,7 +3089,7 @@
         <v>6897</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
@@ -3000,7 +3097,7 @@
         <v>7006</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
@@ -3008,7 +3105,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
@@ -3016,7 +3113,7 @@
         <v>6823</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>74</v>
       </c>
@@ -3024,7 +3121,7 @@
         <v>6790</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>75</v>
       </c>
@@ -3032,7 +3129,7 @@
         <v>6981</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>76</v>
       </c>
@@ -3040,7 +3137,7 @@
         <v>7080</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>77</v>
       </c>
@@ -3048,7 +3145,7 @@
         <v>6954</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>78</v>
       </c>
@@ -3056,7 +3153,7 @@
         <v>6843</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>79</v>
       </c>
@@ -3064,7 +3161,7 @@
         <v>7107</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>80</v>
       </c>
@@ -3072,7 +3169,7 @@
         <v>6941</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>81</v>
       </c>
@@ -3080,7 +3177,7 @@
         <v>6906</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>82</v>
       </c>
@@ -3088,7 +3185,7 @@
         <v>6758</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
@@ -3096,7 +3193,7 @@
         <v>6841</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
@@ -3104,7 +3201,7 @@
         <v>6906</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>85</v>
       </c>
@@ -3112,7 +3209,7 @@
         <v>6755</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>86</v>
       </c>
@@ -3120,7 +3217,7 @@
         <v>6888</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>87</v>
       </c>
@@ -3128,7 +3225,7 @@
         <v>7021</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>88</v>
       </c>
@@ -3136,7 +3233,7 @@
         <v>6630</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>89</v>
       </c>
@@ -3144,7 +3241,7 @@
         <v>6811</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>90</v>
       </c>
@@ -3152,7 +3249,7 @@
         <v>6725</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
@@ -3160,7 +3257,7 @@
         <v>6675</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
@@ -3168,7 +3265,7 @@
         <v>6756</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
@@ -3176,7 +3273,7 @@
         <v>6732</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
@@ -3184,7 +3281,7 @@
         <v>6714</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
@@ -3192,7 +3289,7 @@
         <v>7084</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
@@ -3200,7 +3297,7 @@
         <v>6833</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>97</v>
       </c>
@@ -3208,7 +3305,7 @@
         <v>6736</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>98</v>
       </c>
@@ -3216,7 +3313,7 @@
         <v>7185</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>99</v>
       </c>
@@ -3224,7 +3321,7 @@
         <v>6969</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>100</v>
       </c>
@@ -3232,7 +3329,7 @@
         <v>6539</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>101</v>
       </c>
@@ -3240,7 +3337,7 @@
         <v>6730</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>102</v>
       </c>
@@ -3248,7 +3345,7 @@
         <v>6860</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>103</v>
       </c>
@@ -3256,7 +3353,7 @@
         <v>6912</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>104</v>
       </c>
@@ -3264,7 +3361,7 @@
         <v>6856</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>105</v>
       </c>
@@ -3272,7 +3369,7 @@
         <v>6866</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>106</v>
       </c>
@@ -3280,7 +3377,7 @@
         <v>6887</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>108</v>
       </c>
@@ -3288,7 +3385,7 @@
         <v>6796</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>109</v>
       </c>
@@ -3296,7 +3393,7 @@
         <v>7020</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>110</v>
       </c>
@@ -3304,7 +3401,7 @@
         <v>7189</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>111</v>
       </c>
@@ -3312,7 +3409,7 @@
         <v>6902</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>112</v>
       </c>
@@ -3320,7 +3417,7 @@
         <v>6856</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>113</v>
       </c>
@@ -3328,7 +3425,7 @@
         <v>6836</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>114</v>
       </c>
@@ -3336,7 +3433,7 @@
         <v>7126</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>115</v>
       </c>
@@ -3344,7 +3441,7 @@
         <v>6847</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>116</v>
       </c>
@@ -3352,7 +3449,7 @@
         <v>7196</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>117</v>
       </c>
@@ -3360,7 +3457,7 @@
         <v>6946</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>118</v>
       </c>
@@ -3368,7 +3465,7 @@
         <v>6754</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>119</v>
       </c>
@@ -3376,7 +3473,7 @@
         <v>6790</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>121</v>
       </c>
@@ -3384,7 +3481,7 @@
         <v>6733</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>122</v>
       </c>
@@ -3392,7 +3489,7 @@
         <v>7168</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>123</v>
       </c>
@@ -3400,7 +3497,7 @@
         <v>6823</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>124</v>
       </c>
@@ -3408,7 +3505,7 @@
         <v>7133</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>125</v>
       </c>
@@ -3416,7 +3513,7 @@
         <v>6815</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>126</v>
       </c>
@@ -3424,7 +3521,7 @@
         <v>6756</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>127</v>
       </c>
@@ -3432,7 +3529,7 @@
         <v>7132</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>128</v>
       </c>
@@ -3440,7 +3537,7 @@
         <v>7011</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>129</v>
       </c>
@@ -3448,7 +3545,7 @@
         <v>6637</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>130</v>
       </c>
@@ -3456,7 +3553,7 @@
         <v>7683</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>131</v>
       </c>
@@ -3464,7 +3561,7 @@
         <v>6884</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>132</v>
       </c>
@@ -3472,7 +3569,7 @@
         <v>6750</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>133</v>
       </c>
@@ -3480,7 +3577,7 @@
         <v>7174</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>134</v>
       </c>
@@ -3488,7 +3585,7 @@
         <v>6640</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>135</v>
       </c>
@@ -3496,7 +3593,7 @@
         <v>6868</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>136</v>
       </c>
@@ -3504,7 +3601,7 @@
         <v>6812</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>137</v>
       </c>
@@ -3512,7 +3609,7 @@
         <v>6809</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>138</v>
       </c>
@@ -3520,7 +3617,7 @@
         <v>7070</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>139</v>
       </c>
@@ -3528,7 +3625,7 @@
         <v>6868</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>140</v>
       </c>
@@ -3536,7 +3633,7 @@
         <v>7152</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>141</v>
       </c>
@@ -3544,7 +3641,7 @@
         <v>7066</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>142</v>
       </c>
@@ -3552,7 +3649,7 @@
         <v>7483</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>143</v>
       </c>
@@ -3560,7 +3657,7 @@
         <v>7244</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>144</v>
       </c>
@@ -3568,7 +3665,7 @@
         <v>6991</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>145</v>
       </c>
@@ -3576,7 +3673,7 @@
         <v>6598</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>146</v>
       </c>
@@ -3584,7 +3681,7 @@
         <v>7201</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>147</v>
       </c>
@@ -3592,7 +3689,7 @@
         <v>6777</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>148</v>
       </c>
@@ -3600,7 +3697,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>149</v>
       </c>
@@ -3608,7 +3705,7 @@
         <v>7051</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>150</v>
       </c>
@@ -3616,7 +3713,7 @@
         <v>7113</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>151</v>
       </c>
@@ -3624,7 +3721,7 @@
         <v>7060</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>152</v>
       </c>
@@ -3632,7 +3729,7 @@
         <v>7111</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>153</v>
       </c>
@@ -3640,7 +3737,7 @@
         <v>6901</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>155</v>
       </c>
@@ -3648,7 +3745,7 @@
         <v>7505</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>156</v>
       </c>
@@ -3656,7 +3753,7 @@
         <v>6654</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>157</v>
       </c>
@@ -3664,7 +3761,7 @@
         <v>7165</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>158</v>
       </c>
@@ -3672,7 +3769,7 @@
         <v>6760</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>159</v>
       </c>
@@ -3680,7 +3777,7 @@
         <v>7232</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>160</v>
       </c>
@@ -3688,7 +3785,7 @@
         <v>7247</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>161</v>
       </c>
@@ -3696,7 +3793,7 @@
         <v>7260</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>162</v>
       </c>
@@ -3704,7 +3801,7 @@
         <v>7012</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>163</v>
       </c>
@@ -3712,7 +3809,7 @@
         <v>7086</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>164</v>
       </c>
@@ -3720,7 +3817,7 @@
         <v>7315</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>165</v>
       </c>
@@ -3728,7 +3825,7 @@
         <v>7198</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>166</v>
       </c>
@@ -3736,7 +3833,7 @@
         <v>7549</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>167</v>
       </c>
@@ -3744,7 +3841,7 @@
         <v>7249</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>168</v>
       </c>
@@ -3752,7 +3849,7 @@
         <v>7316</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>169</v>
       </c>
@@ -3760,7 +3857,7 @@
         <v>6978</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>170</v>
       </c>
@@ -3768,7 +3865,7 @@
         <v>7187</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>171</v>
       </c>
@@ -3776,7 +3873,7 @@
         <v>7346</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>172</v>
       </c>
@@ -3784,7 +3881,7 @@
         <v>6984</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>173</v>
       </c>
@@ -3792,7 +3889,7 @@
         <v>7743</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>174</v>
       </c>
@@ -3800,7 +3897,7 @@
         <v>6995</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>175</v>
       </c>
@@ -3808,7 +3905,7 @@
         <v>7281</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>176</v>
       </c>
@@ -3816,7 +3913,7 @@
         <v>6991</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>177</v>
       </c>
@@ -3824,7 +3921,7 @@
         <v>7004</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>178</v>
       </c>
@@ -3832,7 +3929,7 @@
         <v>6950</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>179</v>
       </c>
@@ -3840,7 +3937,7 @@
         <v>7002</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>181</v>
       </c>
@@ -3848,7 +3945,7 @@
         <v>7028</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>182</v>
       </c>
@@ -3856,7 +3953,7 @@
         <v>7061</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>183</v>
       </c>
@@ -3864,7 +3961,7 @@
         <v>6957</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>184</v>
       </c>
@@ -3872,7 +3969,7 @@
         <v>7245</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>185</v>
       </c>
@@ -3880,7 +3977,7 @@
         <v>7063</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>186</v>
       </c>
@@ -3888,7 +3985,7 @@
         <v>6947</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>187</v>
       </c>
@@ -3896,7 +3993,7 @@
         <v>7939</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>188</v>
       </c>
@@ -3904,7 +4001,7 @@
         <v>6956</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>189</v>
       </c>
@@ -3919,24 +4016,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>